<commit_message>
Changed the column names
</commit_message>
<xml_diff>
--- a/Multi-Level-Spreadsheet.xlsx
+++ b/Multi-Level-Spreadsheet.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1461578744.ctr\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="8160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,10 +33,10 @@
     <t>Miscellaneous</t>
   </si>
   <si>
-    <t>Portland</t>
+    <t>Ghana</t>
   </si>
   <si>
-    <t>Vancouver</t>
+    <t>Nigeria</t>
   </si>
 </sst>
 </file>
@@ -139,7 +134,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -174,7 +169,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -351,7 +346,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -362,16 +357,16 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>